<commit_message>
Far east fed. dist. 13-14 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/cities15-16/7/d1.xlsx
+++ b/migforecasting/cities15-16/7/d1.xlsx
@@ -469,12 +469,13 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>